<commit_message>
Tried prompts on Mistral and LLaMA
</commit_message>
<xml_diff>
--- a/Cisco exam/Cisco CCNA practice test.XLSX
+++ b/Cisco exam/Cisco CCNA practice test.XLSX
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\algar\Documents\Travail\Research assistant\GitHub\ChatGPTExperiments\Cisco exam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0E259B-0E48-42B1-9B51-46F9F6048DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A95B5B6-663B-4C7B-9E58-00A604D74458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChatGPT" sheetId="9" r:id="rId1"/>
     <sheet name="Bard" sheetId="12" r:id="rId2"/>
-    <sheet name="Mistral" sheetId="10" r:id="rId3"/>
-    <sheet name="Llama" sheetId="11" r:id="rId4"/>
+    <sheet name="Mistral" sheetId="14" r:id="rId3"/>
+    <sheet name="LLaMA" sheetId="13" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,373 +39,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="123">
   <si>
     <t>CORRECT ANSWER</t>
   </si>
   <si>
-    <t>A, B, E</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>B, C, E</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>B, D</t>
-  </si>
-  <si>
     <t>ZERO-SHOT PROMPT</t>
   </si>
   <si>
-    <t>A, E</t>
-  </si>
-  <si>
     <t>Answer</t>
   </si>
   <si>
-    <t>### Answer the proposed question. Make sure you read the entire question, since some of them may or may not tell you how many options you must choose ###
-Question: Which three statements are true about the operation of a full-duplex Ethernet network? (Choose three.)
-Options: 
-A. There are no collisions in full-duplex mode.
-B. A dedicated switch port is required for each full-duplex node.
-C. Ethernet hub ports are preconfigured for full-duplex mode.
-D. In a full-duplex environment, the host network card must check for the availability of
-the network media before transmitting.
-E. The host network card and the switch port must be capable of operating in full-duplex
-mode
-Answer:</t>
-  </si>
-  <si>
-    <t>### Answer the proposed question. Make sure you read the entire question, since some of them may or may not tell you how many options you must choose ###
-Question: Which layer of the TCP/IP stack combines the OSI model physical and data link layers?
-Options:
-A. Internet layer
-B. Transport layer
-C. Application layer
-D. Network access layer
-Answer:</t>
-  </si>
-  <si>
-    <t>### Answer the proposed question. Make sure you read the entire question, since some of them may or may not tell you how many options you must choose ###
-Question: Which protocol uses a connection-oriented service to deliver files between end systems?
-Options:
-A. TFTP
-B. DNS
-C. FTP
-D. SNMP
-E. RIP
-Answer:</t>
-  </si>
-  <si>
-    <t>### Answer the proposed question. Make sure you read the entire question, since some of them may or may not tell you how many options you must choose ###
-Question: Which statements accurately describe CDP? (Choose three.)
-Options: 
-A. CDP is an IEEE standard protocol.
-B. CDP is a Cisco proprietary protocol.
-C. CDP is a datalink layer protocol.
-D. CDP is a network layer protocol.
-E. CDP can discover directly connected neighboring Cisco devices.
-F. CDP can discover Cisco devices that are not directly connected
-Answer:</t>
-  </si>
-  <si>
-    <t>### Answer the proposed question. Make sure you read the entire question, since some of them may or may not tell you how many options you must choose ###
-Question: How does a switch differ from a hub?
-Options:
-A. A switch does not induce any latency into the frame transfer time.
-B. A switch tracks MAC addresses of directly-connected devices.
-C. A switch operates at a lower, more efficient layer of the OSI model.
-D. A switch decreases the number of broadcast domains.
-E. A switch decreases the number of collision domains.
-Answer:</t>
-  </si>
-  <si>
-    <t>### Answer the proposed question. Make sure you read the entire question, since some of them may or may not tell you how many options you must choose ###
-Question: What must occur before a workstation can exchange HTTP packets with a web server?
-Options:
-A. A UDP connection must be established between the workstation and its default
-gateway.
-B. A UDP connection must be established between the workstation and the web server.
-C. A TCP connection must be established between the workstation and its default gateway.
-D. A TCP connection must be established between the workstation and the web server.
-E. An ICMP connection must be established between the workstation and its default
-gateway.
-F. An ICMP connection must be established between the workstation and the web server.
-Answer:</t>
-  </si>
-  <si>
-    <t>### Answer the proposed question. Make sure you read the entire question, since some of them may or may not tell you how many options you must choose ###
-Question: How does TCP differ from UDP? (Choose two.)
-Options:
-A. TCP provides best effort delivery.
-B. TCP provides synchronized communication.
-C. TCP segments are essentially datagrams.
-D. TCP provides sequence numbering of packets.
-E. TCP uses broadcast delivery.
-Answer:</t>
-  </si>
-  <si>
-    <t>### Answer the proposed question. Make sure you read the entire question, since some of them may or may not tell you how many options you must choose ###
-Question: Which layer of the OSI model controls the reliability of communications between network devices using flow control, sequencing and acknowledgments?
-Options:
-A. Physical
-B. Data-link
-C. Transport
-D. Network
-Answer:</t>
-  </si>
-  <si>
     <t>ZERO-SHOT COT PROMPT</t>
   </si>
   <si>
-    <t>Which three statements are true about the operation of a full-duplex Ethernet network? (Choose three.)
-A. There are no collisions in full-duplex mode.
-B. A dedicated switch port is required for each full-duplex node.
-C. Ethernet hub ports are preconfigured for full-duplex mode.
-D. In a full-duplex environment, the host network card must check for the availability of
-the network media before transmitting.
-E. The host network card and the switch port must be capable of operating in full-duplex
-mode
-Let's think step by step</t>
-  </si>
-  <si>
     <t>Reasoning</t>
-  </si>
-  <si>
-    <t>### Answer the proposed question. Make sure you read the entire question, since some of them may or may not tell you how many options you must choose ###
-Question: Which OSI layer header contains the address of a destination host that is on another network?
-Options: 
-A. Application
-B. Session
-C. Transport
-D. Network
-E. Data link
-F. Physical
-Answer:</t>
-  </si>
-  <si>
-    <t>Which OSI layer header contains the address of a destination host that is on another network?
-A. Application
-B. Session
-C. Transport
-D. Network
-E. Data link
-F. Physical
-Let's think step by step</t>
-  </si>
-  <si>
-    <t>Which layer of the TCP/IP stack combines the OSI model physical and data link layers?
-A. Internet layer
-B. Transport layer
-C. Application layer
-D. Network access layer
-Let's think step by step</t>
-  </si>
-  <si>
-    <t>Which protocol uses a connection-oriented service to deliver files between end systems?
-A. TFTP
-B. DNS
-C. FTP
-D. SNMP
-E. RIP
-Let's think step by step</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Which statements accurately describe CDP? (Choose three.)
-A. CDP is an IEEE standard protocol.
-B. CDP is a Cisco proprietary protocol.
-C. CDP is a datalink layer protocol.
-D. CDP is a network layer protocol.
-E. CDP can discover directly connected neighboring Cisco devices.
-F. CDP can discover Cisco devices that are not directly connected
-Let's think step by step</t>
-  </si>
-  <si>
-    <t>How does a switch differ from a hub?
-A. A switch does not induce any latency into the frame transfer time.
-B. A switch tracks MAC addresses of directly-connected devices.
-C. A switch operates at a lower, more efficient layer of the OSI model.
-D. A switch decreases the number of broadcast domains.
-E. A switch decreases the number of collision domains.
-Let's think step by step</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What must occur before a workstation can exchange HTTP packets with a web server?
-A. A UDP connection must be established between the workstation and its default
-gateway.
-B. A UDP connection must be established between the workstation and the web server.
-C. A TCP connection must be established between the workstation and its default gateway.
-D. A TCP connection must be established between the workstation and the web server.
-E. An ICMP connection must be established between the workstation and its default
-gateway.
-F. An ICMP connection must be established between the workstation and the web server.
-Let's think step by step </t>
-  </si>
-  <si>
-    <t>How does TCP differ from UDP? (Choose two.)
-A. TCP provides best effort delivery.
-B. TCP provides synchronized communication.
-C. TCP segments are essentially datagrams.
-D. TCP provides sequence numbering of packets.
-E. TCP uses broadcast delivery.
-Let's think step by step</t>
-  </si>
-  <si>
-    <t>Which layer of the OSI model controls the reliability of communications between network devices using flow control, sequencing and acknowledgments?
-A. Physical
-B. Data-link
-C. Transport
-D. Network
-Let's think step by step</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>A, D</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>A, E, D</t>
-  </si>
-  <si>
-    <t>B, E, F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sure! Let's go through the options one by one:
-A. There are no collisions in full-duplex mode.
-True. In full-duplex mode, each device can transmit and receive simultaneously, so there is no possibility of collisions occurring.
-B. A dedicated switch port is required for each full-duplex node.
-False. A dedicated switch port is not required for each full-duplex node. Full-duplex nodes can share a switch port with other nodes, as long as the switch port is capable of operating in full-duplex mode.
-C. Ethernet hub ports are preconfigured for full-duplex mode.
-False. Ethernet hub ports are not preconfigured for full-duplex mode. In fact, Ethernet hubs do not support full-duplex mode at all.
-D. In a full-duplex environment, the host network card must check for the availability of the network media before transmitting.
-False. In a full-duplex environment, the host network card does not need to check for the availability of the network media before transmitting. This is because the switch port is capable of operating in full-duplex mode, which means that it can simultaneously transmit and receive data.
-E. The host network card and the switch port must be capable of operating in full-duplex mode.
-True. The host network card and the switch port must be capable of operating in full-duplex mode in order for the network to operate in full-duplex mode.
-</t>
-  </si>
-  <si>
-    <t>Sure! Let's go through the options one by one:
-A. Application
-The Application layer header does not contain the address of a destination host that is on another network. The Application layer is responsible for providing services to end-user applications, such as email, file transfer, and remote login. It does not concern itself with network-to-network communication.
-B. Session
-The Session layer header does not contain the address of a destination host that is on another network. The Session layer is responsible for establishing, maintaining, and terminating connections between applications. It does not provide any information about the network-to-network communication.
-C. Transport
-The Transport layer header contains the address of a destination host that is on another network. The Transport layer is responsible for providing reliable data transfer between devices on different networks. It uses a connection-oriented or connectionless protocol to ensure that data is delivered reliably. The destination host address is included in the Transport layer header to enable the data to be routed to the correct device on the destination network.
-D. Network
-The Network layer header does not contain the address of a destination host that is on another network. The Network layer is responsible for routing data between different networks. It uses a routing table to determine the best path for data to travel from the source network to the destination network. The destination host address is not included in the Network layer header, as it is not concerned with the specific devices on the destination network.
-E. Data link
-The Data link layer header does not contain the address of a destination host that is on another network. The Data link layer is responsible for providing error-free transfer of data between devices on the same network. It does not concern itself with network-to-network communication.
-F. Physical
-The Physical layer header does not contain the address of a destination host that is on another network. The Physical layer is responsible for transmitting raw bits over a physical medium. It does not provide any information about the network-to-network communication.</t>
-  </si>
-  <si>
-    <t>Sure! Let's go through the options one by one:
-A. Internet layer
-The Internet layer does not combine the OSI model physical and data link layers. The Internet layer is responsible for routing data between different networks and providing logical addressing and routing. It does not concern itself with the physical and data link layers.
-B. Transport layer
-The Transport layer does not combine the OSI model physical and data link layers. The Transport layer is responsible for providing reliable data transfer between devices on different networks. It uses a connection-oriented or connectionless protocol to ensure that data is delivered reliably, but it does not concern itself with the physical and data link layers.
-C. Application layer
-The Application layer does not combine the OSI model physical and data link layers. The Application layer is responsible for providing services to end-user applications, such as email, file transfer, and remote login. It does not concern itself with the physical and data link layers.
-D. Network access layer
-The Network access layer combines the OSI model physical and data link layers. The Network access layer is responsible for providing access to the network and for transmitting data over the network. It includes the physical and data link layers of the OSI model, which are responsible for transmitting raw bits over a physical medium and for providing error-free transfer of data between devices on the same network, respectively.</t>
-  </si>
-  <si>
-    <t>Sure! Let's go through the options one by one:
-A. TFTP
-TFTP (Trivial File Transfer Protocol) is a simple file transfer protocol that does not use a connection-oriented service to deliver files between end systems. TFTP is a datagram-based protocol, which means that it does not establish a connection before transmitting data. Instead, it relies on the UDP protocol to handle the transmission of data.
-B. DNS
-DNS (Domain Name System) is a protocol used for resolving domain names to IP addresses. It does not provide a connection-oriented service for delivering files between end systems.
-C. FTP
-FTP (File Transfer Protocol) is a protocol used for transferring files between end systems. It establishes a connection between the client and server before transmitting data, which makes it a connection-oriented protocol. FTP uses a dedicated connection to ensure that data is delivered reliably and in the correct order.
-D. SNMP
-SNMP (Simple Network Management Protocol) is a protocol used for managing and monitoring network devices. It does not provide a connection-oriented service for delivering files between end systems.
-E. RIP
-RIP (Routing Information Protocol) is a distance-vector routing protocol used for routing decisions in a network. It does not provide a connection-oriented service for delivering files between end systems.</t>
-  </si>
-  <si>
-    <t>B, D, E</t>
-  </si>
-  <si>
-    <t>Sure! Let's go through the options one by one:
-A. CDP is an IEEE standard protocol.
-False. CDP (Cisco Discovery Protocol) is a Cisco proprietary protocol, not an IEEE standard protocol.
-B. CDP is a Cisco proprietary protocol.
-True. CDP is a protocol developed by Cisco Systems for discovering and managing Cisco devices on a network.
-C. CDP is a datalink layer protocol.
-False. CDP operates at the network layer, not the datalink layer.
-D. CDP is a network layer protocol.
-True. CDP is a network layer protocol that uses IP packets to discover and communicate with other Cisco devices.
-E. CDP can discover directly connected neighboring Cisco devices.
-True. CDP can discover directly connected neighboring Cisco devices by sending and receiving CDP packets over the network.
-F. CDP can discover Cisco devices that are not directly connected
-False. CDP can only discover devices that are directly connected to the same network as the device running CDP. It cannot discover devices that are not directly connected.</t>
-  </si>
-  <si>
-    <t>Sure! Let's go through the options one by one:
-A. A switch does not induce any latency into the frame transfer time.
-False. Both switches and hubs can introduce latency into the frame transfer time, as they need to process the frames and forward them to the appropriate ports.
-B. A switch tracks MAC addresses of directly-connected devices.
-True. A switch keeps a table of MAC addresses of devices that are directly connected to it, which allows it to forward frames more efficiently. A hub, on the other hand, does not keep track of MAC addresses and simply broadcasts all frames to all ports.
-C. A switch operates at a lower, more efficient layer of the OSI model.
-False. Both switches and hubs operate at the data link layer (Layer 2) of the OSI model.
-D. A switch decreases the number of broadcast domains.
-True. A switch can divide a large broadcast domain into smaller ones, reducing the number of devices that receive broadcast traffic.
-E. A switch decreases the number of collision domains.
-True. A switch can divide a large collision domain into smaller ones, reducing the number of devices that can collide with each other.</t>
-  </si>
-  <si>
-    <t>Sure! Let's go through the options one by one:
-A. A UDP connection must be established between the workstation and its default gateway.
-Not necessary. HTTP uses TCP, not UDP, to establish connections.
-B. A UDP connection must be established between the workstation and the web server.
-Not necessary. As mentioned above, HTTP uses TCP, not UDP, to establish connections.
-C. A TCP connection must be established between the workstation and its default gateway.
-Not necessary. The workstation does not need to establish a TCP connection with its default gateway to access the web server.
-D. A TCP connection must be established between the workstation and the web server.
-Correct! To exchange HTTP packets with the web server, a TCP connection must be established between the workstation and the web server.
-E. An ICMP connection must be established between the workstation and its default gateway.
-Not necessary. ICMP is used for error-reporting and diagnostic functions, not for establishing connections.
-F. An ICMP connection must be established between the workstation and the web server.
-Not necessary. As mentioned above, ICMP is not used for establishing connections.</t>
-  </si>
-  <si>
-    <t>Sure! Let's go through the options one by one:
-A. TCP provides best effort delivery.
-False. TCP provides reliable delivery, which means that it guarantees that data will be delivered correctly and in the order it was sent. It does not provide best effort delivery, which means that it does not guarantee delivery and may drop packets if necessary.
-B. TCP provides synchronized communication.
-False. TCP does not provide synchronized communication. It is a connection-oriented protocol, which means that a connection must be established between the sender and receiver before data can be sent. However, once the connection is established, TCP does not provide any mechanism for synchronizing the sender and receiver.
-C. TCP segments are essentially datagrams.
-False. TCP segments are not datagrams. A datagram is a self-contained unit of data that contains all the information necessary to deliver it to its destination. TCP segments, on the other hand, are fragments of a larger packet that are sent over a connection.
-D. TCP provides sequence numbering of packets.
-True. TCP provides sequence numbering of packets to ensure that data is delivered in the correct order. It assigns a sequence number to each packet and sends it to the receiver, which uses the sequence number to reassemble the packets in the correct order.
-E. TCP uses broadcast delivery.
-False. TCP does not use broadcast delivery. It is a connection-oriented protocol, which means that it establishes a dedicated connection between the sender and receiver before sending data. It does not use broadcast delivery, which means that it does not send data to multiple recipients at once.</t>
-  </si>
-  <si>
-    <t>Sure! Let's go through the options one by one:
-A. Physical
-The Physical layer is responsible for transmitting raw bits over a physical medium. It does not control the reliability of communications between network devices using flow control, sequencing, and acknowledgments.
-B. Data-link
-The Data-link layer provides error-free transfer of data frames between two devices on the same network. It uses flow control and sequencing to ensure that data is transmitted efficiently and in the correct order. However, it does not use acknowledgments to ensure that data is received correctly.
-C. Transport
-The Transport layer is responsible for providing reliable data transfer between devices. It uses flow control, sequencing, and acknowledgments to ensure that data is transmitted reliably and in the correct order. It also provides error detection and correction, and can resend data if it is lost or corrupted.
-D. Network
-The Network layer is responsible for routing data between devices on different networks. It does not control the reliability of communications between network devices using flow control, sequencing, and acknowledgments.</t>
   </si>
   <si>
     <t>### Answer the proposed question. Make sure you read the entire question ###
@@ -1169,6 +820,212 @@
 * **Cisco Express Forwarding (CEF)**: This proprietary forwarding method is similar to cut-through switching in that it begins forwarding frames as soon as the destination MAC address is received. However, CEF uses a number of techniques to reduce the risk of errors, such as performing error checking on the header and trailer of the frame.
 * **Queuing**: This method is not a switching method, but it can be used in conjunction with any of the other methods to improve latency. Queuing allows the switch to prioritize certain types of traffic, such as voice or video, so that these packets are forwarded before other packets.
 Therefore, the correct answer is **Cut-through**. Cut-through switching is the Ethernet switching method that provides the lowest latency, although it comes at the risk of introducing errors.</t>
+  </si>
+  <si>
+    <t>PROMPT</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: Which Rapid Spanning Tree Protocol port state is a combination of standard 802.1D STP's disabled, blocking and listening states?
+Options: 
+Blocking
+Discarding
+Learning
+Forwarding
+Listening
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t>Listening</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: Host A receives a frame and discards it after determining it is corrupt. Which OSI layer checks frames for errors?
+Options: 
+Application
+Network
+Physical
+Data-link
+FCS or CRC
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t>FCS or CRC</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: No matter how it's configured, a single switch port is considered what?
+Options: 
+A separate unicast domain
+A separate broadcast domain
+A separate multicast domain
+A separate collision domain
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: Identify which of the services below uses both TCP and UDP ports.
+Options: 
+FTP
+TFTP
+DNS
+SSH
+Telnet
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: A router with a BGP autonomous system number of 65001 is peered with another router with the same BGP AS. Which of the following is true?
+Options: 
+    The ebgp multihop command must be configured to reach an established state.
+    A BGP connection will be established, but no traffic will traverse the connection.
+    The routers are considered eBGP neighbors.
+    The routers are considered iBGP neighbors.
+    A BGP establishment error will occur because of the AS conflict.
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t>The routers are considered eBGP neighbors.</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: What is the default 802.1D short spanning tree port cost of a 10 Gbps Ethernet link?
+Options: 
+10
+4
+2
+2,000
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[INST] Answer the proposed question. Make sure you read the entire question 
+Question: Which of the following is the correct syntax to configure a switch port as a standard user port on VLAN 10 for data and VLAN 50 for VoIP?
+Options: 
+TechTarget-SW1(config-if)#switchport mode trunk TechTarget-SW1(config-if)#switchport access vlan 10 TechTarget-SW1(config-if)#switchport voice vlan 50
+TechTarget-SW1(config-if)#switchport mode access TechTarget-SW1(config-if)#switchport access vlan 10 TechTarget-SW1(config-if)#switchport voice vlan 50
+TechTarget-SW1(config-if)#switchport mode trunk TechTarget-SW1(config-if)#switchport access vlan 10 TechTarget-SW1(config-if)#switchport voip vlan 50
+TechTarget-SW1(config-if)#switchport mode access TechTarget-SW1(config-if)#switchport access vlan 10 TechTarget-SW1(config-if)#switchport voip vlan 50
+TechTarget-SW1(config-if)#switchport mode access TechTarget-SW1(config-if)#switchport access vlan 50 TechTarget-SW1(config-if)#switchport voice vlan 10
+Just answer without explanations [/INST]
+</t>
+  </si>
+  <si>
+    <t>TechTarget-SW1(config-if)#switchport mode trunk TechTarget-SW1(config-if)#switchport access vlan 10 TechTarget-SW1(config-if)#switchport voice vlan 50</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: One of the routers in your company has just received information about network 172.16.10.0/24 from multiple sources. Which of the below will the router consider as the most reliable source for network 172.16.10.0/24?
+Options: 
+An EIGRP update for network 172.16.10.0/24
+An OSPF update for network 172.16.10.0/24
+A static route to network 172.16.10.0/24
+A default route with a next hop address of 172.16.0.1
+A directly connected interface with an IP address of 172.16.10.254/24
+None of the abovThe router will discard the update.
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: Which of the following options are used in standard access lists?
+Options: 
+    Destination address and subnet mask
+    Source address and subnet mask
+    Destination address and wildcard mask
+    Source address and wildcard mask
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t>Destination address and wildcard amsk</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: When configuring NAT, what is the purpose of the overload command, as used in the following example:
+Router(config)#ip nat inside source list 1 interface gi0/2 overload
+Options: 
+It translates a single local address into many global addresses by tracking the connection's UDP port number.
+It indicates a one-to-one translation on the interface by tracking the connection's TCP port number.
+It translates many local addresses into a single global address by tracking the connection's TCP port number.
+It translates a single local address into many global addresses by tracking the connection's TCP port number.
+It translates many local addresses into a single global address by tracking the connection's UDP port number.
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: Which statement about NTP is true?
+Options: 
+A stratum 2 NTP server is directly attached to an authoritative time source.
+NTP must be configured to synchronize with one of a handful of atomic clocks available on the internet.
+NTP authentication is disabled by default.
+You must configure two or more NTP sources for times to be accurat
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: What would the result be when the following commands are executed on a Cisco Catalyst switch:
+TechTarget-SW1 (config-if)# switchport port-security
+TechTarget-SW1 (config-if)# switchport port-security mac-address sticky
+Options: 
+The MAC address learned dynamically is saved in the switch's running-configuration.
+The MAC address learned dynamically is saved in the switch's startup configuration.
+The MAC address learned dynamically is saved permanently in the VLAN database.
+The statically configured MAC address is saved in the switch's running configuration when frames from that address are received.
+The first MAC address seen on the specific port is allowed to access the network until the port security timer expires.
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t>The first MAC address seen on the specific port is allowed to access the network until the port security timer expires</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: Which of the following is not an IPv6 address type?
+Options: 
+Broadcast
+Unicast
+Anycast
+Multicast
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t>Anycast</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: A router has two identical default routes to 10.0.0.0/24. One route is learned via EIGRP, and the other is a static route. Which of the following commands will set the static route so it's only used in the event the EIGRP route is no longer available?
+Options: 
+ip route 10.0.0.0 255.0.0.0 192.168.1.254 10
+ip route 10.0.0.0 255.0.0.0 192.168.1.254 100
+ip route 10.0.0.0 255.0.0.0 192.168.1.254 distance 10
+ip route 10.0.0.0 255.0.0.0 192.168.1.254 distance 100 
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t>[INST] Answer the proposed question. Make sure you read the entire question 
+Question: Which Ethernet switching method would you use if low latency is of utmost importance?
+Options: 
+First-in-first-out
+Store-and-forward
+Cut-through
+Cisco Express Forwarding (CEF)
+Queuing
+Just answer without explanations [/INST]</t>
+  </si>
+  <si>
+    <t>TFTP</t>
+  </si>
+  <si>
+    <t>A BGP establishment error will occur because of the AS conflict.</t>
+  </si>
+  <si>
+    <t>An EIGRP update for network 172.16.10.0/24</t>
+  </si>
+  <si>
+    <t>Destination address and subnet mask</t>
+  </si>
+  <si>
+    <t>It translates a single local address into many global addresses by tracking the connection's UDP port number.</t>
+  </si>
+  <si>
+    <t>You must configure two or more NTP sources for times to be accurate.</t>
   </si>
 </sst>
 </file>
@@ -1296,21 +1153,7 @@
     <cellStyle name="60% - Énfasis6" xfId="3" builtinId="52"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -1688,7 +1531,7 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="72" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1705,19 +1548,19 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>0</v>
@@ -1726,116 +1569,116 @@
     </row>
     <row r="2" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="303.60000000000002" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="358.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="E7" s="3">
         <v>2</v>
@@ -1846,301 +1689,301 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="345" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="372.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" ht="248.4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="276" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="317.39999999999998" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="386.4" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B21">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>B2&lt;&gt;F2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>B2=F2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E21">
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>E2&lt;&gt;F2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>E2=F2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2170,19 +2013,19 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>0</v>
@@ -2191,116 +2034,116 @@
     </row>
     <row r="2" spans="1:7" ht="317.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="207" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="345" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="276" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="E7" s="3">
         <v>2</v>
@@ -2311,785 +2154,289 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" ht="207" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>124</v>
+        <v>84</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="234.6" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B21">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>B2&lt;&gt;F2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>B2=F2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E21">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>E2&lt;&gt;F2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>E2=F2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A7DE89-4722-482C-A770-36DEF3580BCF}">
-  <sheetPr codeName="Hoja6"/>
-  <dimension ref="A1:G11"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="55.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="55.88671875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="66.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="10"/>
-    </row>
-    <row r="2" spans="1:7" ht="262.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="234.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="193.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="207" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="220.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="220.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="193.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="207" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:B11">
-    <cfRule type="expression" dxfId="13" priority="1">
-      <formula>B2&lt;&gt;F2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
-      <formula>B2=F2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E11">
-    <cfRule type="expression" dxfId="11" priority="3">
-      <formula>E2&lt;&gt;F2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
-      <formula>E2=F2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B1D2C2-C7B0-4E6D-9BB0-AB8006C3B3D6}">
-  <sheetPr codeName="Hoja7"/>
-  <dimension ref="A1:G11"/>
-  <sheetViews>
-    <sheetView zoomScale="73" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="55.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="55.88671875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="66.109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="10"/>
-    </row>
-    <row r="2" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="400.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="372.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:B11">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>B2&lt;&gt;F2</formula>
     </cfRule>
@@ -3097,7 +2444,7 @@
       <formula>B2=F2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E11">
+  <conditionalFormatting sqref="E2:E21">
     <cfRule type="expression" dxfId="7" priority="3">
       <formula>E2&lt;&gt;F2</formula>
     </cfRule>
@@ -3108,4 +2455,531 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB97319-954D-403C-A489-F706FA5E6A92}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="55.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4" ht="207" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="248.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="358.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="248.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="276" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="207" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="1:4" ht="303.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="207" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B21">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>B2&lt;&gt;C2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>B2=C2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63719041-6776-4EF2-99AC-C097A2BB221D}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="55.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4" ht="207" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="248.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="358.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="248.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="276" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="207" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="1:4" ht="303.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="207" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B21">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>B2&lt;&gt;C2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>B2=C2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a count to know the number of correct results
</commit_message>
<xml_diff>
--- a/Cisco exam/Cisco CCNA practice test.XLSX
+++ b/Cisco exam/Cisco CCNA practice test.XLSX
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\algar\Documents\Travail\Research assistant\GitHub\ChatGPTExperiments\Cisco exam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\algar\Documents\Travail\Research assistant\GitHub\LLMExperiments\Cisco exam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A95B5B6-663B-4C7B-9E58-00A604D74458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5C3C34-5EA3-436C-9B3E-0277D91D27EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChatGPT" sheetId="9" r:id="rId1"/>
@@ -39,12 +39,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="126">
   <si>
     <t>CORRECT ANSWER</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>ZERO-SHOT PROMPT</t>
@@ -1026,6 +1023,18 @@
   </si>
   <si>
     <t>You must configure two or more NTP sources for times to be accurate.</t>
+  </si>
+  <si>
+    <t>Preguntas acertadas</t>
+  </si>
+  <si>
+    <t>Preguntas acertadas (ZERO-SHOT)</t>
+  </si>
+  <si>
+    <t>Preguntas acertadas (ZERO-SHOT COT)</t>
+  </si>
+  <si>
+    <t>Preguntas totales</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1110,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1137,15 +1146,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Énfasis1" xfId="1" builtinId="32"/>
@@ -1153,21 +1153,7 @@
     <cellStyle name="60% - Énfasis6" xfId="3" builtinId="52"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1531,8 +1517,8 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView zoomScale="72" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1548,19 +1534,19 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>0</v>
@@ -1569,116 +1555,116 @@
     </row>
     <row r="2" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="303.60000000000002" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="C4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="358.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="E6" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="E7" s="3">
         <v>2</v>
@@ -1687,303 +1673,244 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>1</v>
+    <row r="8" spans="1:7" ht="345" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="345" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>1</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="372.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" ht="193.2" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="248.4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="372.6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="276" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
-        <v>1</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="317.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="1:7" ht="248.4" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="276" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="317.39999999999998" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>1</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="386.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="220.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="386.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="3">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B21">
-    <cfRule type="expression" dxfId="13" priority="1">
+  <conditionalFormatting sqref="B2:B17">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>B2&lt;&gt;F2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>B2=F2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E21">
-    <cfRule type="expression" dxfId="11" priority="3">
+  <conditionalFormatting sqref="E2:E17">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>E2&lt;&gt;F2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>E2=F2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1996,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A609C18-5F54-4BFC-A8AC-80164A3FCF57}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A17" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2013,19 +1940,19 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>0</v>
@@ -2034,116 +1961,116 @@
     </row>
     <row r="2" spans="1:7" ht="317.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="207" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="345" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="276" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="3">
         <v>2</v>
@@ -2152,303 +2079,244 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>1</v>
+    <row r="8" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="207" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>82</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>1</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" ht="207" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
-        <v>1</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="1:7" ht="220.8" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="234.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>1</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="234.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="3">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B21">
-    <cfRule type="expression" dxfId="9" priority="1">
+  <conditionalFormatting sqref="B2:B17">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>B2&lt;&gt;F2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>B2=F2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E21">
-    <cfRule type="expression" dxfId="7" priority="3">
+  <conditionalFormatting sqref="E2:E17">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>E2&lt;&gt;F2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>E2=F2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2459,10 +2327,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB97319-954D-403C-A489-F706FA5E6A92}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A17" zoomScale="91" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2475,10 +2343,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -2487,62 +2355,62 @@
     </row>
     <row r="2" spans="1:4" ht="207" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="248.4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -2551,169 +2419,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>1</v>
+    <row r="8" spans="1:4" ht="358.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="358.8" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>104</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="248.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>1</v>
-      </c>
       <c r="B10" s="3" t="s">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="248.4" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="276" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
-        <v>1</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="207" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="303.60000000000002" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="276" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="207" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" ht="303.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="165.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="207" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>37</v>
+      <c r="B19" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="3">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B21">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="B2:B17">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>B2&lt;&gt;C2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>B2=C2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2724,10 +2561,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63719041-6776-4EF2-99AC-C097A2BB221D}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A17" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2740,10 +2577,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -2752,62 +2589,62 @@
     </row>
     <row r="2" spans="1:4" ht="207" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="248.4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -2816,166 +2653,135 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>1</v>
+    <row r="8" spans="1:4" ht="358.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="358.8" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="248.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>1</v>
-      </c>
       <c r="B10" s="3" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>106</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="248.4" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="276" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
-        <v>1</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="207" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="303.60000000000002" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="276" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="207" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>1</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" ht="303.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="165.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="207" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="3">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B21">
-    <cfRule type="expression" dxfId="3" priority="3">
+  <conditionalFormatting sqref="B2:B17">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>B2&lt;&gt;C2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>B2=C2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added counter of correct answers
</commit_message>
<xml_diff>
--- a/Cisco exam/Cisco CCNA practice test.XLSX
+++ b/Cisco exam/Cisco CCNA practice test.XLSX
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\algar\Documents\Travail\Research assistant\GitHub\LLMExperiments\Cisco exam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5C3C34-5EA3-436C-9B3E-0277D91D27EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261B3780-11BE-4ED4-BE7E-69774F749C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChatGPT" sheetId="9" r:id="rId1"/>
@@ -1148,9 +1148,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="60% - Énfasis1" xfId="1" builtinId="32"/>
-    <cellStyle name="60% - Énfasis2" xfId="2" builtinId="36"/>
-    <cellStyle name="60% - Énfasis6" xfId="3" builtinId="52"/>
+    <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
+    <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
+    <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
@@ -1517,11 +1517,11 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A17" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="55.77734375" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.44140625" style="3" customWidth="1"/>
@@ -1927,7 +1927,7 @@
       <selection activeCell="A19" sqref="A19:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="55.77734375" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.44140625" style="3" customWidth="1"/>
@@ -2329,11 +2329,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB97319-954D-403C-A489-F706FA5E6A92}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="91" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="55.77734375" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.88671875" style="3" customWidth="1"/>
@@ -2567,7 +2567,7 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="55.77734375" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.88671875" style="3" customWidth="1"/>

</xml_diff>